<commit_message>
Can write the first EML file now as well
</commit_message>
<xml_diff>
--- a/doc/Test status.xlsx
+++ b/doc/Test status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="14220"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
   <si>
     <t>Test status</t>
   </si>
@@ -75,13 +75,16 @@
   </si>
   <si>
     <t>Write as format, read back in, compare</t>
+  </si>
+  <si>
+    <t>hdr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,8 +114,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,6 +140,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -239,11 +254,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -301,9 +317,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -585,7 +605,7 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,7 +898,9 @@
       <c r="C16" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="13"/>
+      <c r="E16" s="33" t="s">
+        <v>17</v>
+      </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -955,7 +977,7 @@
       <c r="S19" s="19"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -980,10 +1002,11 @@
       <c r="S21" s="26"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1008,6 +1031,7 @@
       <c r="S23" s="29"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" t="s">
         <v>4</v>
@@ -1028,10 +1052,11 @@
       <c r="S24" s="32"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B26" s="2" t="s">

</xml_diff>

<commit_message>
Cross of 3 inputs to 3 inputs tested
</commit_message>
<xml_diff>
--- a/doc/Test status.xlsx
+++ b/doc/Test status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="14220"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="27870" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
   <si>
     <t>Test status</t>
   </si>
@@ -77,7 +77,19 @@
     <t>Write as format, read back in, compare</t>
   </si>
   <si>
-    <t>hdr</t>
+    <t>H, N8</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Incomplete header (source has too little information).</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Limitation to 8 characters in input names.</t>
   </si>
 </sst>
 </file>
@@ -259,7 +271,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -318,6 +330,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -602,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S27"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,7 +711,7 @@
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="J6" s="7"/>
       <c r="K6" s="9"/>
       <c r="M6" s="14"/>
       <c r="N6" s="15"/>
@@ -735,7 +753,7 @@
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="J8" s="7"/>
       <c r="K8" s="9"/>
       <c r="M8" s="14"/>
       <c r="N8" s="15"/>
@@ -898,14 +916,14 @@
       <c r="C16" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="33"/>
+      <c r="F16" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
+      <c r="J16" s="7"/>
       <c r="K16" s="9"/>
       <c r="M16" s="14"/>
       <c r="N16" s="15"/>
@@ -1099,6 +1117,22 @@
       <c r="R27" s="31"/>
       <c r="S27" s="32"/>
     </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
RBX code compiles (untested)
</commit_message>
<xml_diff>
--- a/doc/Test status.xlsx
+++ b/doc/Test status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="27870" windowHeight="14220"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="27870" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
   <si>
     <t>Test status</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>Limitation to 8 characters in input names.</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>"All pass" sometimes, sometimes not</t>
+  </si>
+  <si>
+    <t>H,N8,A</t>
   </si>
 </sst>
 </file>
@@ -620,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,7 +718,9 @@
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="H6" s="35" t="s">
+        <v>22</v>
+      </c>
       <c r="I6" s="8"/>
       <c r="J6" s="7"/>
       <c r="K6" s="9"/>
@@ -751,7 +762,9 @@
       <c r="E8" s="6"/>
       <c r="F8" s="7"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="H8" s="35" t="s">
+        <v>22</v>
+      </c>
       <c r="I8" s="8"/>
       <c r="J8" s="7"/>
       <c r="K8" s="9"/>
@@ -832,12 +845,14 @@
       <c r="C12" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="H12" s="35" t="s">
+        <v>22</v>
+      </c>
       <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+      <c r="J12" s="7"/>
       <c r="K12" s="9"/>
       <c r="M12" s="14"/>
       <c r="N12" s="15"/>
@@ -921,7 +936,9 @@
         <v>17</v>
       </c>
       <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
+      <c r="H16" s="35" t="s">
+        <v>24</v>
+      </c>
       <c r="I16" s="8"/>
       <c r="J16" s="7"/>
       <c r="K16" s="9"/>
@@ -1133,6 +1150,38 @@
         <v>21</v>
       </c>
     </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="34"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="34"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="34"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="34"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="34"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="34"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="34"/>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="34"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
RBX works for read and write
</commit_message>
<xml_diff>
--- a/doc/Test status.xlsx
+++ b/doc/Test status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="0" windowWidth="27870" windowHeight="14220"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="27870" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="26">
   <si>
     <t>Test status</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>H,N8,A</t>
+  </si>
+  <si>
+    <t>RBX</t>
   </si>
 </sst>
 </file>
@@ -632,7 +635,7 @@
   <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,7 +643,7 @@
     <col min="2" max="2" width="5.875" customWidth="1"/>
     <col min="3" max="3" width="6.125" customWidth="1"/>
     <col min="4" max="4" width="3.625" customWidth="1"/>
-    <col min="5" max="11" width="5.625" style="3" customWidth="1"/>
+    <col min="5" max="11" width="6" style="3" customWidth="1"/>
     <col min="12" max="12" width="3.625" customWidth="1"/>
     <col min="13" max="19" width="5.625" customWidth="1"/>
   </cols>
@@ -675,7 +678,7 @@
         <v>8</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>10</v>
@@ -721,7 +724,9 @@
       <c r="H6" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="8"/>
+      <c r="I6" s="35" t="s">
+        <v>22</v>
+      </c>
       <c r="J6" s="7"/>
       <c r="K6" s="9"/>
       <c r="M6" s="14"/>
@@ -765,7 +770,9 @@
       <c r="H8" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="8"/>
+      <c r="I8" s="35" t="s">
+        <v>22</v>
+      </c>
       <c r="J8" s="7"/>
       <c r="K8" s="9"/>
       <c r="M8" s="14"/>
@@ -851,7 +858,9 @@
       <c r="H12" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="8"/>
+      <c r="I12" s="35" t="s">
+        <v>22</v>
+      </c>
       <c r="J12" s="7"/>
       <c r="K12" s="9"/>
       <c r="M12" s="14"/>
@@ -884,17 +893,19 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
+      <c r="H14" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
       <c r="K14" s="9"/>
       <c r="M14" s="14"/>
       <c r="N14" s="15"/>
@@ -939,7 +950,9 @@
       <c r="H16" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="8"/>
+      <c r="I16" s="35" t="s">
+        <v>24</v>
+      </c>
       <c r="J16" s="7"/>
       <c r="K16" s="9"/>
       <c r="M16" s="14"/>

</xml_diff>

<commit_message>
Reads the RP LIN file, dies while writing LIN, may not write others properly
</commit_message>
<xml_diff>
--- a/doc/Test status.xlsx
+++ b/doc/Test status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="27870" windowHeight="14220"/>
+    <workbookView xWindow="6510" yWindow="0" windowWidth="27870" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="29">
   <si>
     <t>Test status</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>RBX</t>
+  </si>
+  <si>
+    <t>LIN_RP</t>
+  </si>
+  <si>
+    <t>LIN_VG</t>
+  </si>
+  <si>
+    <t>LIN_TRN</t>
   </si>
 </sst>
 </file>
@@ -146,7 +155,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,6 +178,12 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -283,7 +298,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -350,6 +365,12 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -632,36 +653,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:Y43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.875" customWidth="1"/>
+    <col min="2" max="2" width="7.75" customWidth="1"/>
     <col min="3" max="3" width="6.125" customWidth="1"/>
     <col min="4" max="4" width="3.625" customWidth="1"/>
-    <col min="5" max="11" width="6" style="3" customWidth="1"/>
-    <col min="12" max="12" width="3.625" customWidth="1"/>
-    <col min="13" max="19" width="5.625" customWidth="1"/>
+    <col min="5" max="14" width="7.25" style="3" customWidth="1"/>
+    <col min="15" max="15" width="3.625" customWidth="1"/>
+    <col min="16" max="25" width="7.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -675,40 +696,58 @@
         <v>7</v>
       </c>
       <c r="H5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="P5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="S5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="W5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="X5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="Y5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -720,44 +759,56 @@
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="35" t="s">
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="35" t="s">
+      <c r="L6" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="9"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="9"/>
+      <c r="P6" s="14"/>
       <c r="Q6" s="15"/>
       <c r="R6" s="15"/>
-      <c r="S6" s="16"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="16"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
       <c r="J7" s="11"/>
-      <c r="K7" s="12"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="12"/>
+      <c r="P7" s="17"/>
       <c r="Q7" s="18"/>
       <c r="R7" s="18"/>
-      <c r="S7" s="19"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S7" s="18"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="18"/>
+      <c r="V7" s="18"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="19"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
@@ -766,86 +817,110 @@
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="35" t="s">
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="35" t="s">
+      <c r="L8" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="9"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="9"/>
+      <c r="P8" s="14"/>
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
-      <c r="S8" s="16"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="16"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
       <c r="J9" s="11"/>
-      <c r="K9" s="12"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="12"/>
+      <c r="P9" s="17"/>
       <c r="Q9" s="18"/>
       <c r="R9" s="18"/>
-      <c r="S9" s="19"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="19"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
       <c r="J10" s="8"/>
-      <c r="K10" s="9"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="9"/>
+      <c r="P10" s="14"/>
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
-      <c r="S10" s="16"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="16"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
       <c r="J11" s="11"/>
-      <c r="K11" s="12"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="12"/>
+      <c r="P11" s="17"/>
       <c r="Q11" s="18"/>
       <c r="R11" s="18"/>
-      <c r="S11" s="19"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S11" s="18"/>
+      <c r="T11" s="18"/>
+      <c r="U11" s="18"/>
+      <c r="V11" s="18"/>
+      <c r="W11" s="18"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="19"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
@@ -854,44 +929,56 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="35" t="s">
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="35" t="s">
+      <c r="L12" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="9"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="9"/>
+      <c r="P12" s="14"/>
       <c r="Q12" s="15"/>
       <c r="R12" s="15"/>
-      <c r="S12" s="16"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="16"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
       <c r="J13" s="11"/>
-      <c r="K13" s="12"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="12"/>
+      <c r="P13" s="17"/>
       <c r="Q13" s="18"/>
       <c r="R13" s="18"/>
-      <c r="S13" s="19"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S13" s="18"/>
+      <c r="T13" s="18"/>
+      <c r="U13" s="18"/>
+      <c r="V13" s="18"/>
+      <c r="W13" s="18"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="19"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>25</v>
       </c>
@@ -900,42 +987,54 @@
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="35" t="s">
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="9"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="9"/>
+      <c r="P14" s="14"/>
       <c r="Q14" s="15"/>
       <c r="R14" s="15"/>
-      <c r="S14" s="16"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="16"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
       <c r="J15" s="11"/>
-      <c r="K15" s="12"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="12"/>
+      <c r="P15" s="17"/>
       <c r="Q15" s="18"/>
       <c r="R15" s="18"/>
-      <c r="S15" s="19"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="19"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
@@ -946,44 +1045,56 @@
       <c r="F16" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="35" t="s">
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="35" t="s">
+      <c r="L16" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="9"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="16"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M16" s="7"/>
+      <c r="N16" s="9"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="37"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="37"/>
+      <c r="U16" s="37"/>
+      <c r="V16" s="37"/>
+      <c r="W16" s="37"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="38"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
       <c r="J17" s="11"/>
-      <c r="K17" s="12"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="19"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="12"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="40"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="40"/>
+      <c r="T17" s="40"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="40"/>
+      <c r="W17" s="40"/>
+      <c r="X17" s="18"/>
+      <c r="Y17" s="41"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
@@ -992,39 +1103,51 @@
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
       <c r="J18" s="8"/>
-      <c r="K18" s="9"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="16"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="9"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="37"/>
+      <c r="S18" s="37"/>
+      <c r="T18" s="37"/>
+      <c r="U18" s="37"/>
+      <c r="V18" s="37"/>
+      <c r="W18" s="37"/>
+      <c r="X18" s="37"/>
+      <c r="Y18" s="16"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
       <c r="J19" s="11"/>
-      <c r="K19" s="12"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="19"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="12"/>
+      <c r="P19" s="39"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="40"/>
+      <c r="T19" s="40"/>
+      <c r="U19" s="40"/>
+      <c r="V19" s="40"/>
+      <c r="W19" s="40"/>
+      <c r="X19" s="40"/>
+      <c r="Y19" s="19"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
@@ -1040,22 +1163,28 @@
       <c r="H21" s="22"/>
       <c r="I21" s="22"/>
       <c r="J21" s="22"/>
-      <c r="K21" s="23"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="25"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="23"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="22"/>
       <c r="R21" s="25"/>
-      <c r="S21" s="26"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S21" s="25"/>
+      <c r="T21" s="25"/>
+      <c r="U21" s="25"/>
+      <c r="V21" s="25"/>
+      <c r="W21" s="25"/>
+      <c r="X21" s="25"/>
+      <c r="Y21" s="26"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>7</v>
@@ -1069,16 +1198,22 @@
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
-      <c r="K23" s="16"/>
-      <c r="M23" s="27"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="28"/>
-      <c r="P23" s="28"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="16"/>
+      <c r="P23" s="27"/>
       <c r="Q23" s="28"/>
-      <c r="R23" s="28"/>
-      <c r="S23" s="29"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R23" s="15"/>
+      <c r="S23" s="28"/>
+      <c r="T23" s="28"/>
+      <c r="U23" s="28"/>
+      <c r="V23" s="28"/>
+      <c r="W23" s="28"/>
+      <c r="X23" s="28"/>
+      <c r="Y23" s="29"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" t="s">
@@ -1090,110 +1225,184 @@
       <c r="H24" s="18"/>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
-      <c r="K24" s="19"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="31"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="19"/>
+      <c r="P24" s="30"/>
       <c r="Q24" s="31"/>
-      <c r="R24" s="31"/>
-      <c r="S24" s="32"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R24" s="18"/>
+      <c r="S24" s="31"/>
+      <c r="T24" s="31"/>
+      <c r="U24" s="31"/>
+      <c r="V24" s="31"/>
+      <c r="W24" s="31"/>
+      <c r="X24" s="31"/>
+      <c r="Y24" s="32"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C26" t="s">
         <v>3</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="15"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="8"/>
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
-      <c r="K26" s="16"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="28"/>
-      <c r="O26" s="28"/>
-      <c r="P26" s="28"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="16"/>
+      <c r="P26" s="27"/>
       <c r="Q26" s="28"/>
       <c r="R26" s="28"/>
-      <c r="S26" s="29"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S26" s="15"/>
+      <c r="T26" s="28"/>
+      <c r="U26" s="28"/>
+      <c r="V26" s="28"/>
+      <c r="W26" s="28"/>
+      <c r="X26" s="28"/>
+      <c r="Y26" s="29"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>4</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="18"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="11"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
-      <c r="K27" s="19"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="31"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="19"/>
+      <c r="P27" s="30"/>
       <c r="Q27" s="31"/>
       <c r="R27" s="31"/>
-      <c r="S27" s="32"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S27" s="18"/>
+      <c r="T27" s="31"/>
+      <c r="U27" s="31"/>
+      <c r="V27" s="31"/>
+      <c r="W27" s="31"/>
+      <c r="X27" s="31"/>
+      <c r="Y27" s="32"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="14"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="16"/>
+      <c r="P29" s="27"/>
+      <c r="Q29" s="28"/>
+      <c r="R29" s="28"/>
+      <c r="S29" s="28"/>
+      <c r="T29" s="15"/>
+      <c r="U29" s="28"/>
+      <c r="V29" s="28"/>
+      <c r="W29" s="28"/>
+      <c r="X29" s="28"/>
+      <c r="Y29" s="29"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="19"/>
+      <c r="P30" s="30"/>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="31"/>
+      <c r="S30" s="31"/>
+      <c r="T30" s="18"/>
+      <c r="U30" s="31"/>
+      <c r="V30" s="31"/>
+      <c r="W30" s="31"/>
+      <c r="X30" s="31"/>
+      <c r="Y30" s="32"/>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="34" t="s">
+      <c r="E33" s="34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E34" s="34" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>22</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E35" s="34" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33" s="34"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E34" s="34"/>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E35" s="34"/>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E36" s="34"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E37" s="34"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E38" s="34"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E39" s="34"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E40" s="34"/>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="34"/>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="34"/>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E43" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Small fixes mostly to team carry
</commit_message>
<xml_diff>
--- a/doc/Test status.xlsx
+++ b/doc/Test status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="0" windowWidth="27870" windowHeight="14220"/>
+    <workbookView xWindow="7440" yWindow="0" windowWidth="27870" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="35">
   <si>
     <t>Test status</t>
   </si>
@@ -111,6 +111,24 @@
   </si>
   <si>
     <t>LIN_TRN</t>
+  </si>
+  <si>
+    <t>DLE</t>
+  </si>
+  <si>
+    <t>DLE,A</t>
+  </si>
+  <si>
+    <t>TEK,N8</t>
+  </si>
+  <si>
+    <t>TEK</t>
+  </si>
+  <si>
+    <t>Incomplete with respect to Date, Location, Event</t>
+  </si>
+  <si>
+    <t>Incomplete with respect to Title, Event, Teams</t>
   </si>
 </sst>
 </file>
@@ -656,7 +674,7 @@
   <dimension ref="A1:Y43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="V30" sqref="V30"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,7 +780,7 @@
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
-      <c r="J6" s="8"/>
+      <c r="J6" s="7"/>
       <c r="K6" s="35" t="s">
         <v>22</v>
       </c>
@@ -820,7 +838,7 @@
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
-      <c r="J8" s="8"/>
+      <c r="J8" s="7"/>
       <c r="K8" s="35" t="s">
         <v>22</v>
       </c>
@@ -873,15 +891,23 @@
       <c r="C10" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="8"/>
+      <c r="E10" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>29</v>
+      </c>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="7"/>
       <c r="N10" s="9"/>
       <c r="P10" s="14"/>
       <c r="Q10" s="15"/>
@@ -932,7 +958,7 @@
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
-      <c r="J12" s="8"/>
+      <c r="J12" s="7"/>
       <c r="K12" s="35" t="s">
         <v>22</v>
       </c>
@@ -990,7 +1016,7 @@
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
-      <c r="J14" s="8"/>
+      <c r="J14" s="7"/>
       <c r="K14" s="35" t="s">
         <v>22</v>
       </c>
@@ -1048,7 +1074,9 @@
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
-      <c r="J16" s="8"/>
+      <c r="J16" s="35" t="s">
+        <v>31</v>
+      </c>
       <c r="K16" s="35" t="s">
         <v>24</v>
       </c>
@@ -1381,10 +1409,20 @@
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E36" s="34"/>
+      <c r="C36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="34" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E37" s="34"/>
+      <c r="C37" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="34" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E38" s="34"/>

</xml_diff>

<commit_message>
Reads first REC file
</commit_message>
<xml_diff>
--- a/doc/Test status.xlsx
+++ b/doc/Test status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="0" windowWidth="27870" windowHeight="14220"/>
+    <workbookView xWindow="8370" yWindow="0" windowWidth="27870" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
   <si>
     <t>Test status</t>
   </si>
@@ -129,6 +129,18 @@
   </si>
   <si>
     <t>Incomplete with respect to Title, Event, Teams</t>
+  </si>
+  <si>
+    <t>H, P</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Not all tricks of play are shown</t>
+  </si>
+  <si>
+    <t>H,A,P</t>
   </si>
 </sst>
 </file>
@@ -316,7 +328,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -348,9 +360,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -674,7 +683,7 @@
   <dimension ref="A1:Y43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,28 +786,28 @@
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="35" t="s">
+      <c r="K6" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="35" t="s">
+      <c r="L6" s="34" t="s">
         <v>22</v>
       </c>
       <c r="M6" s="7"/>
       <c r="N6" s="9"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="16"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="15"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
@@ -807,24 +816,24 @@
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
       <c r="N7" s="12"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="19"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="18"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -835,28 +844,28 @@
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
       <c r="J8" s="7"/>
-      <c r="K8" s="35" t="s">
+      <c r="K8" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="35" t="s">
+      <c r="L8" s="34" t="s">
         <v>22</v>
       </c>
       <c r="M8" s="7"/>
       <c r="N8" s="9"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="16"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="15"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
@@ -865,24 +874,24 @@
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
       <c r="N9" s="12"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18"/>
-      <c r="W9" s="18"/>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="19"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="17"/>
+      <c r="Y9" s="18"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
@@ -891,34 +900,34 @@
       <c r="C10" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="35" t="s">
+      <c r="K10" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="L10" s="35" t="s">
+      <c r="L10" s="34" t="s">
         <v>29</v>
       </c>
       <c r="M10" s="7"/>
       <c r="N10" s="9"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="16"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="15"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
@@ -927,24 +936,24 @@
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
       <c r="N11" s="12"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="19"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="18"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
@@ -955,28 +964,28 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="35" t="s">
+      <c r="K12" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="35" t="s">
+      <c r="L12" s="34" t="s">
         <v>22</v>
       </c>
       <c r="M12" s="7"/>
       <c r="N12" s="9"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="15"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="16"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="15"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
@@ -985,24 +994,24 @@
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
       <c r="N13" s="12"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="19"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="17"/>
+      <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
@@ -1013,26 +1022,26 @@
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="35" t="s">
+      <c r="K14" s="34" t="s">
         <v>22</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
       <c r="N14" s="9"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="16"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="15"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
@@ -1041,24 +1050,24 @@
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
       <c r="N15" s="12"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18"/>
-      <c r="W15" s="18"/>
-      <c r="X15" s="18"/>
-      <c r="Y15" s="19"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="18"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
@@ -1067,34 +1076,34 @@
       <c r="C16" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="35" t="s">
+      <c r="E16" s="32"/>
+      <c r="F16" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="35" t="s">
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="K16" s="35" t="s">
+      <c r="K16" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="35" t="s">
+      <c r="L16" s="34" t="s">
         <v>24</v>
       </c>
       <c r="M16" s="7"/>
       <c r="N16" s="9"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="37"/>
-      <c r="R16" s="37"/>
-      <c r="S16" s="37"/>
-      <c r="T16" s="37"/>
-      <c r="U16" s="37"/>
-      <c r="V16" s="37"/>
-      <c r="W16" s="37"/>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="38"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="36"/>
+      <c r="S16" s="36"/>
+      <c r="T16" s="36"/>
+      <c r="U16" s="36"/>
+      <c r="V16" s="36"/>
+      <c r="W16" s="36"/>
+      <c r="X16" s="14"/>
+      <c r="Y16" s="37"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
@@ -1103,24 +1112,24 @@
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="11"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
       <c r="N17" s="12"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="40"/>
-      <c r="R17" s="40"/>
-      <c r="S17" s="40"/>
-      <c r="T17" s="40"/>
-      <c r="U17" s="40"/>
-      <c r="V17" s="40"/>
-      <c r="W17" s="40"/>
-      <c r="X17" s="18"/>
-      <c r="Y17" s="41"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="39"/>
+      <c r="S17" s="39"/>
+      <c r="T17" s="39"/>
+      <c r="U17" s="39"/>
+      <c r="V17" s="39"/>
+      <c r="W17" s="39"/>
+      <c r="X17" s="17"/>
+      <c r="Y17" s="40"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
@@ -1129,26 +1138,38 @@
       <c r="C18" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
+      <c r="E18" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="M18" s="34" t="s">
+        <v>36</v>
+      </c>
       <c r="N18" s="9"/>
-      <c r="P18" s="36"/>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="37"/>
-      <c r="S18" s="37"/>
-      <c r="T18" s="37"/>
-      <c r="U18" s="37"/>
-      <c r="V18" s="37"/>
-      <c r="W18" s="37"/>
-      <c r="X18" s="37"/>
-      <c r="Y18" s="16"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="36"/>
+      <c r="U18" s="36"/>
+      <c r="V18" s="36"/>
+      <c r="W18" s="36"/>
+      <c r="X18" s="36"/>
+      <c r="Y18" s="15"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
@@ -1156,24 +1177,24 @@
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="11"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
       <c r="N19" s="12"/>
-      <c r="P19" s="39"/>
-      <c r="Q19" s="40"/>
-      <c r="R19" s="40"/>
-      <c r="S19" s="40"/>
-      <c r="T19" s="40"/>
-      <c r="U19" s="40"/>
-      <c r="V19" s="40"/>
-      <c r="W19" s="40"/>
-      <c r="X19" s="40"/>
-      <c r="Y19" s="19"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="39"/>
+      <c r="R19" s="39"/>
+      <c r="S19" s="39"/>
+      <c r="T19" s="39"/>
+      <c r="U19" s="39"/>
+      <c r="V19" s="39"/>
+      <c r="W19" s="39"/>
+      <c r="X19" s="39"/>
+      <c r="Y19" s="18"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -1185,26 +1206,26 @@
       <c r="C21" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="23"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="22"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="25"/>
-      <c r="T21" s="25"/>
-      <c r="U21" s="25"/>
-      <c r="V21" s="25"/>
-      <c r="W21" s="25"/>
-      <c r="X21" s="25"/>
-      <c r="Y21" s="26"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="22"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="24"/>
+      <c r="W21" s="24"/>
+      <c r="X21" s="24"/>
+      <c r="Y21" s="25"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
@@ -1220,26 +1241,26 @@
       <c r="C23" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="14"/>
       <c r="G23" s="8"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="16"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="28"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="28"/>
-      <c r="T23" s="28"/>
-      <c r="U23" s="28"/>
-      <c r="V23" s="28"/>
-      <c r="W23" s="28"/>
-      <c r="X23" s="28"/>
-      <c r="Y23" s="29"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="15"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="27"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="27"/>
+      <c r="T23" s="27"/>
+      <c r="U23" s="27"/>
+      <c r="V23" s="27"/>
+      <c r="W23" s="27"/>
+      <c r="X23" s="27"/>
+      <c r="Y23" s="28"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
@@ -1247,26 +1268,26 @@
       <c r="C24" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="18"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="17"/>
       <c r="G24" s="11"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="19"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="31"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="31"/>
-      <c r="T24" s="31"/>
-      <c r="U24" s="31"/>
-      <c r="V24" s="31"/>
-      <c r="W24" s="31"/>
-      <c r="X24" s="31"/>
-      <c r="Y24" s="32"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="18"/>
+      <c r="P24" s="29"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="30"/>
+      <c r="V24" s="30"/>
+      <c r="W24" s="30"/>
+      <c r="X24" s="30"/>
+      <c r="Y24" s="31"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
@@ -1282,51 +1303,51 @@
       <c r="C26" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
       <c r="H26" s="8"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="16"/>
-      <c r="P26" s="27"/>
-      <c r="Q26" s="28"/>
-      <c r="R26" s="28"/>
-      <c r="S26" s="15"/>
-      <c r="T26" s="28"/>
-      <c r="U26" s="28"/>
-      <c r="V26" s="28"/>
-      <c r="W26" s="28"/>
-      <c r="X26" s="28"/>
-      <c r="Y26" s="29"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="15"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="27"/>
+      <c r="S26" s="14"/>
+      <c r="T26" s="27"/>
+      <c r="U26" s="27"/>
+      <c r="V26" s="27"/>
+      <c r="W26" s="27"/>
+      <c r="X26" s="27"/>
+      <c r="Y26" s="28"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="17"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
       <c r="H27" s="11"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="19"/>
-      <c r="P27" s="30"/>
-      <c r="Q27" s="31"/>
-      <c r="R27" s="31"/>
-      <c r="S27" s="18"/>
-      <c r="T27" s="31"/>
-      <c r="U27" s="31"/>
-      <c r="V27" s="31"/>
-      <c r="W27" s="31"/>
-      <c r="X27" s="31"/>
-      <c r="Y27" s="32"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="18"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="30"/>
+      <c r="R27" s="30"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="30"/>
+      <c r="U27" s="30"/>
+      <c r="V27" s="30"/>
+      <c r="W27" s="30"/>
+      <c r="X27" s="30"/>
+      <c r="Y27" s="31"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -1338,57 +1359,57 @@
       <c r="C29" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="14"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
       <c r="J29" s="8"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="16"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="28"/>
-      <c r="R29" s="28"/>
-      <c r="S29" s="28"/>
-      <c r="T29" s="15"/>
-      <c r="U29" s="28"/>
-      <c r="V29" s="28"/>
-      <c r="W29" s="28"/>
-      <c r="X29" s="28"/>
-      <c r="Y29" s="29"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="15"/>
+      <c r="P29" s="26"/>
+      <c r="Q29" s="27"/>
+      <c r="R29" s="27"/>
+      <c r="S29" s="27"/>
+      <c r="T29" s="14"/>
+      <c r="U29" s="27"/>
+      <c r="V29" s="27"/>
+      <c r="W29" s="27"/>
+      <c r="X29" s="27"/>
+      <c r="Y29" s="28"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
       <c r="J30" s="11"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="19"/>
-      <c r="P30" s="30"/>
-      <c r="Q30" s="31"/>
-      <c r="R30" s="31"/>
-      <c r="S30" s="31"/>
-      <c r="T30" s="18"/>
-      <c r="U30" s="31"/>
-      <c r="V30" s="31"/>
-      <c r="W30" s="31"/>
-      <c r="X30" s="31"/>
-      <c r="Y30" s="32"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="18"/>
+      <c r="P30" s="29"/>
+      <c r="Q30" s="30"/>
+      <c r="R30" s="30"/>
+      <c r="S30" s="30"/>
+      <c r="T30" s="17"/>
+      <c r="U30" s="30"/>
+      <c r="V30" s="30"/>
+      <c r="W30" s="30"/>
+      <c r="X30" s="30"/>
+      <c r="Y30" s="31"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="34" t="s">
+      <c r="E33" s="33" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1396,7 +1417,7 @@
       <c r="C34" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="34" t="s">
+      <c r="E34" s="33" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1404,7 +1425,7 @@
       <c r="C35" t="s">
         <v>22</v>
       </c>
-      <c r="E35" s="34" t="s">
+      <c r="E35" s="33" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1412,7 +1433,7 @@
       <c r="C36" t="s">
         <v>29</v>
       </c>
-      <c r="E36" s="34" t="s">
+      <c r="E36" s="33" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1420,27 +1441,32 @@
       <c r="C37" t="s">
         <v>32</v>
       </c>
-      <c r="E37" s="34" t="s">
+      <c r="E37" s="33" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E38" s="34"/>
+      <c r="C38" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="33" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E39" s="34"/>
+      <c r="E39" s="33"/>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E40" s="34"/>
+      <c r="E40" s="33"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E41" s="34"/>
+      <c r="E41" s="33"/>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E42" s="34"/>
+      <c r="E42" s="33"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E43" s="34"/>
+      <c r="E43" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fileREC reads and writes first file
</commit_message>
<xml_diff>
--- a/doc/Test status.xlsx
+++ b/doc/Test status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="0" windowWidth="27870" windowHeight="14220"/>
+    <workbookView xWindow="9300" yWindow="0" windowWidth="27870" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
   <si>
     <t>Test status</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>TXT</t>
-  </si>
-  <si>
-    <t>PBX</t>
   </si>
   <si>
     <t>EML</t>
@@ -328,7 +325,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -348,9 +345,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -398,6 +392,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -683,7 +685,7 @@
   <dimension ref="A1:Y43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,10 +705,10 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -723,25 +725,25 @@
         <v>7</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="P5" s="4" t="s">
         <v>5</v>
@@ -753,25 +755,25 @@
         <v>7</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="V5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="W5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="X5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="X5" s="4" t="s">
+      <c r="Y5" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="Y5" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -786,54 +788,56 @@
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="34" t="s">
-        <v>22</v>
+      <c r="K6" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="33" t="s">
+        <v>21</v>
       </c>
       <c r="M6" s="7"/>
-      <c r="N6" s="9"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14"/>
-      <c r="W6" s="14"/>
-      <c r="X6" s="14"/>
-      <c r="Y6" s="15"/>
+      <c r="N6" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="42"/>
+      <c r="S6" s="42"/>
+      <c r="T6" s="42"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="42"/>
+      <c r="W6" s="42"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="36"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="12"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="17"/>
-      <c r="V7" s="17"/>
-      <c r="W7" s="17"/>
-      <c r="X7" s="17"/>
-      <c r="Y7" s="18"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="11"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="43"/>
+      <c r="S7" s="43"/>
+      <c r="T7" s="43"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="43"/>
+      <c r="W7" s="43"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="39"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -844,116 +848,120 @@
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
       <c r="J8" s="7"/>
-      <c r="K8" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="34" t="s">
-        <v>22</v>
+      <c r="K8" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="33" t="s">
+        <v>21</v>
       </c>
       <c r="M8" s="7"/>
-      <c r="N8" s="9"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="15"/>
+      <c r="N8" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="42"/>
+      <c r="S8" s="42"/>
+      <c r="T8" s="42"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="42"/>
+      <c r="W8" s="42"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="36"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="12"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="17"/>
-      <c r="V9" s="17"/>
-      <c r="W9" s="17"/>
-      <c r="X9" s="17"/>
-      <c r="Y9" s="18"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="11"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="43"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="43"/>
+      <c r="W9" s="43"/>
+      <c r="X9" s="16"/>
+      <c r="Y9" s="39"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" s="34" t="s">
-        <v>29</v>
+      <c r="L10" s="33" t="s">
+        <v>28</v>
       </c>
       <c r="M10" s="7"/>
-      <c r="N10" s="9"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="14"/>
-      <c r="V10" s="14"/>
-      <c r="W10" s="14"/>
-      <c r="X10" s="14"/>
-      <c r="Y10" s="15"/>
+      <c r="N10" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="35"/>
+      <c r="R10" s="35"/>
+      <c r="S10" s="35"/>
+      <c r="T10" s="35"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="35"/>
+      <c r="W10" s="35"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="36"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="12"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="17"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="17"/>
-      <c r="X11" s="17"/>
-      <c r="Y11" s="18"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="11"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="38"/>
+      <c r="T11" s="38"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="38"/>
+      <c r="W11" s="38"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="39"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
@@ -964,241 +972,247 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="L12" s="34" t="s">
-        <v>22</v>
+      <c r="K12" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="33" t="s">
+        <v>21</v>
       </c>
       <c r="M12" s="7"/>
-      <c r="N12" s="9"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="14"/>
-      <c r="X12" s="14"/>
-      <c r="Y12" s="15"/>
+      <c r="N12" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="35"/>
+      <c r="T12" s="35"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="35"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="36"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="12"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="17"/>
-      <c r="U13" s="17"/>
-      <c r="V13" s="17"/>
-      <c r="W13" s="17"/>
-      <c r="X13" s="17"/>
-      <c r="Y13" s="18"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="11"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="38"/>
+      <c r="S13" s="38"/>
+      <c r="T13" s="38"/>
+      <c r="U13" s="16"/>
+      <c r="V13" s="38"/>
+      <c r="W13" s="16"/>
+      <c r="X13" s="16"/>
+      <c r="Y13" s="39"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="34" t="s">
-        <v>22</v>
+      <c r="K14" s="33" t="s">
+        <v>21</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
-      <c r="N14" s="9"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="14"/>
-      <c r="Y14" s="15"/>
+      <c r="N14" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="35"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="35"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="35"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="36"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="12"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="17"/>
-      <c r="U15" s="17"/>
-      <c r="V15" s="17"/>
-      <c r="W15" s="17"/>
-      <c r="X15" s="17"/>
-      <c r="Y15" s="18"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="11"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="38"/>
+      <c r="S15" s="38"/>
+      <c r="T15" s="38"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="38"/>
+      <c r="W15" s="16"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="39"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="32"/>
-      <c r="F16" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="K16" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="L16" s="34" t="s">
-        <v>24</v>
+      <c r="E16" s="31"/>
+      <c r="F16" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="K16" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" s="33" t="s">
+        <v>23</v>
       </c>
       <c r="M16" s="7"/>
-      <c r="N16" s="9"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="36"/>
-      <c r="R16" s="36"/>
-      <c r="S16" s="36"/>
-      <c r="T16" s="36"/>
-      <c r="U16" s="36"/>
-      <c r="V16" s="36"/>
-      <c r="W16" s="36"/>
-      <c r="X16" s="14"/>
-      <c r="Y16" s="37"/>
+      <c r="N16" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="35"/>
+      <c r="R16" s="35"/>
+      <c r="S16" s="35"/>
+      <c r="T16" s="35"/>
+      <c r="U16" s="35"/>
+      <c r="V16" s="35"/>
+      <c r="W16" s="35"/>
+      <c r="X16" s="13"/>
+      <c r="Y16" s="36"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="12"/>
-      <c r="P17" s="38"/>
-      <c r="Q17" s="39"/>
-      <c r="R17" s="39"/>
-      <c r="S17" s="39"/>
-      <c r="T17" s="39"/>
-      <c r="U17" s="39"/>
-      <c r="V17" s="39"/>
-      <c r="W17" s="39"/>
-      <c r="X17" s="17"/>
-      <c r="Y17" s="40"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="11"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
+      <c r="S17" s="38"/>
+      <c r="T17" s="38"/>
+      <c r="U17" s="38"/>
+      <c r="V17" s="38"/>
+      <c r="W17" s="38"/>
+      <c r="X17" s="16"/>
+      <c r="Y17" s="39"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="L18" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="K18" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="L18" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="M18" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="N18" s="9"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="36"/>
-      <c r="R18" s="36"/>
-      <c r="S18" s="36"/>
-      <c r="T18" s="36"/>
-      <c r="U18" s="36"/>
-      <c r="V18" s="36"/>
-      <c r="W18" s="36"/>
-      <c r="X18" s="36"/>
-      <c r="Y18" s="15"/>
+      <c r="N18" s="40"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="35"/>
+      <c r="S18" s="35"/>
+      <c r="T18" s="35"/>
+      <c r="U18" s="35"/>
+      <c r="V18" s="35"/>
+      <c r="W18" s="35"/>
+      <c r="X18" s="35"/>
+      <c r="Y18" s="14"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="12"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="39"/>
-      <c r="R19" s="39"/>
-      <c r="S19" s="39"/>
-      <c r="T19" s="39"/>
-      <c r="U19" s="39"/>
-      <c r="V19" s="39"/>
-      <c r="W19" s="39"/>
-      <c r="X19" s="39"/>
-      <c r="Y19" s="18"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="11"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="38"/>
+      <c r="U19" s="38"/>
+      <c r="V19" s="38"/>
+      <c r="W19" s="38"/>
+      <c r="X19" s="38"/>
+      <c r="Y19" s="17"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>6</v>
@@ -1206,26 +1220,26 @@
       <c r="C21" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="22"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="24"/>
-      <c r="S21" s="24"/>
-      <c r="T21" s="24"/>
-      <c r="U21" s="24"/>
-      <c r="V21" s="24"/>
-      <c r="W21" s="24"/>
-      <c r="X21" s="24"/>
-      <c r="Y21" s="25"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="21"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="23"/>
+      <c r="X21" s="23"/>
+      <c r="Y21" s="24"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
@@ -1233,7 +1247,7 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>7</v>
@@ -1241,26 +1255,26 @@
       <c r="C23" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="14"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="13"/>
       <c r="G23" s="8"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="15"/>
-      <c r="P23" s="26"/>
-      <c r="Q23" s="27"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="27"/>
-      <c r="T23" s="27"/>
-      <c r="U23" s="27"/>
-      <c r="V23" s="27"/>
-      <c r="W23" s="27"/>
-      <c r="X23" s="27"/>
-      <c r="Y23" s="28"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="14"/>
+      <c r="P23" s="25"/>
+      <c r="Q23" s="26"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="26"/>
+      <c r="T23" s="26"/>
+      <c r="U23" s="26"/>
+      <c r="V23" s="26"/>
+      <c r="W23" s="26"/>
+      <c r="X23" s="26"/>
+      <c r="Y23" s="27"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
@@ -1268,26 +1282,26 @@
       <c r="C24" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="18"/>
-      <c r="P24" s="29"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="30"/>
-      <c r="T24" s="30"/>
-      <c r="U24" s="30"/>
-      <c r="V24" s="30"/>
-      <c r="W24" s="30"/>
-      <c r="X24" s="30"/>
-      <c r="Y24" s="31"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="17"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="29"/>
+      <c r="T24" s="29"/>
+      <c r="U24" s="29"/>
+      <c r="V24" s="29"/>
+      <c r="W24" s="29"/>
+      <c r="X24" s="29"/>
+      <c r="Y24" s="30"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
@@ -1295,178 +1309,178 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
       <c r="H26" s="8"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="15"/>
-      <c r="P26" s="26"/>
-      <c r="Q26" s="27"/>
-      <c r="R26" s="27"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="27"/>
-      <c r="U26" s="27"/>
-      <c r="V26" s="27"/>
-      <c r="W26" s="27"/>
-      <c r="X26" s="27"/>
-      <c r="Y26" s="28"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="14"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="26"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="26"/>
+      <c r="U26" s="26"/>
+      <c r="V26" s="26"/>
+      <c r="W26" s="26"/>
+      <c r="X26" s="26"/>
+      <c r="Y26" s="27"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="16"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="18"/>
-      <c r="P27" s="29"/>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="30"/>
-      <c r="S27" s="17"/>
-      <c r="T27" s="30"/>
-      <c r="U27" s="30"/>
-      <c r="V27" s="30"/>
-      <c r="W27" s="30"/>
-      <c r="X27" s="30"/>
-      <c r="Y27" s="31"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="17"/>
+      <c r="P27" s="28"/>
+      <c r="Q27" s="29"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="16"/>
+      <c r="T27" s="29"/>
+      <c r="U27" s="29"/>
+      <c r="V27" s="29"/>
+      <c r="W27" s="29"/>
+      <c r="X27" s="29"/>
+      <c r="Y27" s="30"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
       <c r="J29" s="8"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="15"/>
-      <c r="P29" s="26"/>
-      <c r="Q29" s="27"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="14"/>
-      <c r="U29" s="27"/>
-      <c r="V29" s="27"/>
-      <c r="W29" s="27"/>
-      <c r="X29" s="27"/>
-      <c r="Y29" s="28"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="14"/>
+      <c r="P29" s="25"/>
+      <c r="Q29" s="26"/>
+      <c r="R29" s="26"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="26"/>
+      <c r="V29" s="26"/>
+      <c r="W29" s="26"/>
+      <c r="X29" s="26"/>
+      <c r="Y29" s="27"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="16"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="18"/>
-      <c r="P30" s="29"/>
-      <c r="Q30" s="30"/>
-      <c r="R30" s="30"/>
-      <c r="S30" s="30"/>
-      <c r="T30" s="17"/>
-      <c r="U30" s="30"/>
-      <c r="V30" s="30"/>
-      <c r="W30" s="30"/>
-      <c r="X30" s="30"/>
-      <c r="Y30" s="31"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="17"/>
+      <c r="P30" s="28"/>
+      <c r="Q30" s="29"/>
+      <c r="R30" s="29"/>
+      <c r="S30" s="29"/>
+      <c r="T30" s="16"/>
+      <c r="U30" s="29"/>
+      <c r="V30" s="29"/>
+      <c r="W30" s="29"/>
+      <c r="X30" s="29"/>
+      <c r="Y30" s="30"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="32" t="s">
         <v>18</v>
-      </c>
-      <c r="E33" s="33" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="32" t="s">
         <v>20</v>
-      </c>
-      <c r="E34" s="33" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="32" t="s">
         <v>22</v>
-      </c>
-      <c r="E35" s="33" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E36" s="33" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="E36" s="32" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>32</v>
-      </c>
-      <c r="E37" s="33" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="E37" s="32" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="33" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E39" s="33"/>
+      <c r="E39" s="32"/>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E40" s="33"/>
+      <c r="E40" s="32"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E41" s="33"/>
+      <c r="E41" s="32"/>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E42" s="33"/>
+      <c r="E42" s="32"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E43" s="33"/>
+      <c r="E43" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made a framework for options and Files
</commit_message>
<xml_diff>
--- a/doc/Test status.xlsx
+++ b/doc/Test status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="0" windowWidth="27870" windowHeight="14220"/>
+    <workbookView xWindow="10230" yWindow="0" windowWidth="27870" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="41">
   <si>
     <t>Test status</t>
   </si>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>H,A,P</t>
+  </si>
+  <si>
+    <t>chat, pg</t>
+  </si>
+  <si>
+    <t>chat</t>
+  </si>
+  <si>
+    <t>Commentator chat and pg||'s not matched</t>
   </si>
 </sst>
 </file>
@@ -325,7 +334,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -342,9 +351,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -685,7 +691,7 @@
   <dimension ref="A1:Y43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,56 +794,56 @@
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="33" t="s">
+      <c r="K6" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="33" t="s">
+      <c r="L6" s="32" t="s">
         <v>21</v>
       </c>
       <c r="M6" s="7"/>
-      <c r="N6" s="41" t="s">
+      <c r="N6" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="42"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="42"/>
-      <c r="W6" s="42"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="36"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="41"/>
+      <c r="W6" s="41"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="35"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="11"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="43"/>
-      <c r="S7" s="43"/>
-      <c r="T7" s="43"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="43"/>
-      <c r="W7" s="43"/>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="39"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="10"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="42"/>
+      <c r="S7" s="42"/>
+      <c r="T7" s="42"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="42"/>
+      <c r="W7" s="42"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="38"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -848,56 +854,56 @@
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
       <c r="J8" s="7"/>
-      <c r="K8" s="33" t="s">
+      <c r="K8" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="33" t="s">
+      <c r="L8" s="32" t="s">
         <v>21</v>
       </c>
       <c r="M8" s="7"/>
-      <c r="N8" s="41" t="s">
+      <c r="N8" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="42"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="42"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="42"/>
-      <c r="W8" s="42"/>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="36"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="41"/>
+      <c r="W8" s="41"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="35"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="11"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="43"/>
-      <c r="S9" s="43"/>
-      <c r="T9" s="43"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="43"/>
-      <c r="W9" s="43"/>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="39"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="10"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="42"/>
+      <c r="S9" s="42"/>
+      <c r="T9" s="42"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="42"/>
+      <c r="W9" s="42"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="38"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
@@ -906,62 +912,62 @@
       <c r="C10" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="33" t="s">
+      <c r="K10" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="L10" s="33" t="s">
+      <c r="L10" s="32" t="s">
         <v>28</v>
       </c>
       <c r="M10" s="7"/>
-      <c r="N10" s="41" t="s">
+      <c r="N10" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="35"/>
-      <c r="S10" s="35"/>
-      <c r="T10" s="35"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="35"/>
-      <c r="W10" s="35"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="36"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="34"/>
+      <c r="T10" s="34"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="34"/>
+      <c r="W10" s="34"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="35"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="11"/>
-      <c r="P11" s="37"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="38"/>
-      <c r="U11" s="16"/>
-      <c r="V11" s="38"/>
-      <c r="W11" s="38"/>
-      <c r="X11" s="16"/>
-      <c r="Y11" s="39"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="10"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="37"/>
+      <c r="T11" s="37"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="37"/>
+      <c r="W11" s="37"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="38"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
@@ -972,56 +978,56 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="33" t="s">
+      <c r="K12" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="33" t="s">
+      <c r="L12" s="32" t="s">
         <v>21</v>
       </c>
       <c r="M12" s="7"/>
-      <c r="N12" s="41" t="s">
+      <c r="N12" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="35"/>
-      <c r="T12" s="35"/>
-      <c r="U12" s="13"/>
-      <c r="V12" s="35"/>
-      <c r="W12" s="13"/>
-      <c r="X12" s="13"/>
-      <c r="Y12" s="36"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
+      <c r="T12" s="34"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="34"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="35"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="11"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="38"/>
-      <c r="S13" s="38"/>
-      <c r="T13" s="38"/>
-      <c r="U13" s="16"/>
-      <c r="V13" s="38"/>
-      <c r="W13" s="16"/>
-      <c r="X13" s="16"/>
-      <c r="Y13" s="39"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="10"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="37"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="37"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="38"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
@@ -1032,54 +1038,54 @@
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="33" t="s">
+      <c r="K14" s="32" t="s">
         <v>21</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
-      <c r="N14" s="41" t="s">
+      <c r="N14" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="35"/>
-      <c r="U14" s="13"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="13"/>
-      <c r="X14" s="13"/>
-      <c r="Y14" s="36"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34"/>
+      <c r="T14" s="34"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="34"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="35"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="11"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="38"/>
-      <c r="S15" s="38"/>
-      <c r="T15" s="38"/>
-      <c r="U15" s="16"/>
-      <c r="V15" s="38"/>
-      <c r="W15" s="16"/>
-      <c r="X15" s="16"/>
-      <c r="Y15" s="39"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="10"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="37"/>
+      <c r="T15" s="37"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="37"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="38"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
@@ -1088,62 +1094,62 @@
       <c r="C16" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="33" t="s">
+      <c r="E16" s="30"/>
+      <c r="F16" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="33" t="s">
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="K16" s="33" t="s">
+      <c r="K16" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="L16" s="33" t="s">
+      <c r="L16" s="32" t="s">
         <v>23</v>
       </c>
       <c r="M16" s="7"/>
-      <c r="N16" s="41" t="s">
+      <c r="N16" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="35"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="35"/>
-      <c r="X16" s="13"/>
-      <c r="Y16" s="36"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="34"/>
+      <c r="T16" s="34"/>
+      <c r="U16" s="34"/>
+      <c r="V16" s="34"/>
+      <c r="W16" s="34"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="35"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="11"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="38"/>
-      <c r="R17" s="38"/>
-      <c r="S17" s="38"/>
-      <c r="T17" s="38"/>
-      <c r="U17" s="38"/>
-      <c r="V17" s="38"/>
-      <c r="W17" s="38"/>
-      <c r="X17" s="16"/>
-      <c r="Y17" s="39"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="10"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="37"/>
+      <c r="S17" s="37"/>
+      <c r="T17" s="37"/>
+      <c r="U17" s="37"/>
+      <c r="V17" s="37"/>
+      <c r="W17" s="37"/>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="38"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
@@ -1152,63 +1158,63 @@
       <c r="C18" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="F18" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="33" t="s">
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="K18" s="33" t="s">
+      <c r="K18" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="L18" s="33" t="s">
+      <c r="L18" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="M18" s="33" t="s">
+      <c r="M18" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="N18" s="40"/>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="35"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="35"/>
-      <c r="X18" s="35"/>
-      <c r="Y18" s="14"/>
+      <c r="N18" s="39"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="34"/>
+      <c r="S18" s="34"/>
+      <c r="T18" s="34"/>
+      <c r="U18" s="34"/>
+      <c r="V18" s="34"/>
+      <c r="W18" s="34"/>
+      <c r="X18" s="34"/>
+      <c r="Y18" s="13"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="11"/>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="38"/>
-      <c r="S19" s="38"/>
-      <c r="T19" s="38"/>
-      <c r="U19" s="38"/>
-      <c r="V19" s="38"/>
-      <c r="W19" s="38"/>
-      <c r="X19" s="38"/>
-      <c r="Y19" s="17"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="10"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="37"/>
+      <c r="S19" s="37"/>
+      <c r="T19" s="37"/>
+      <c r="U19" s="37"/>
+      <c r="V19" s="37"/>
+      <c r="W19" s="37"/>
+      <c r="X19" s="37"/>
+      <c r="Y19" s="16"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -1220,26 +1226,26 @@
       <c r="C21" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="21"/>
-      <c r="P21" s="22"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="23"/>
-      <c r="S21" s="23"/>
-      <c r="T21" s="23"/>
-      <c r="U21" s="23"/>
-      <c r="V21" s="23"/>
-      <c r="W21" s="23"/>
-      <c r="X21" s="23"/>
-      <c r="Y21" s="24"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="20"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="22"/>
+      <c r="S21" s="22"/>
+      <c r="T21" s="22"/>
+      <c r="U21" s="22"/>
+      <c r="V21" s="22"/>
+      <c r="W21" s="22"/>
+      <c r="X21" s="22"/>
+      <c r="Y21" s="23"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
@@ -1255,26 +1261,26 @@
       <c r="C23" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="14"/>
-      <c r="P23" s="25"/>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="26"/>
-      <c r="T23" s="26"/>
-      <c r="U23" s="26"/>
-      <c r="V23" s="26"/>
-      <c r="W23" s="26"/>
-      <c r="X23" s="26"/>
-      <c r="Y23" s="27"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="13"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="25"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="25"/>
+      <c r="T23" s="25"/>
+      <c r="U23" s="25"/>
+      <c r="V23" s="25"/>
+      <c r="W23" s="25"/>
+      <c r="X23" s="25"/>
+      <c r="Y23" s="26"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
@@ -1282,26 +1288,26 @@
       <c r="C24" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="17"/>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="29"/>
-      <c r="R24" s="16"/>
-      <c r="S24" s="29"/>
-      <c r="T24" s="29"/>
-      <c r="U24" s="29"/>
-      <c r="V24" s="29"/>
-      <c r="W24" s="29"/>
-      <c r="X24" s="29"/>
-      <c r="Y24" s="30"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="16"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="28"/>
+      <c r="T24" s="28"/>
+      <c r="U24" s="28"/>
+      <c r="V24" s="28"/>
+      <c r="W24" s="28"/>
+      <c r="X24" s="28"/>
+      <c r="Y24" s="29"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
@@ -1317,51 +1323,51 @@
       <c r="C26" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="14"/>
-      <c r="P26" s="25"/>
-      <c r="Q26" s="26"/>
-      <c r="R26" s="26"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="26"/>
-      <c r="U26" s="26"/>
-      <c r="V26" s="26"/>
-      <c r="W26" s="26"/>
-      <c r="X26" s="26"/>
-      <c r="Y26" s="27"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="13"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="25"/>
+      <c r="R26" s="25"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="25"/>
+      <c r="U26" s="25"/>
+      <c r="V26" s="25"/>
+      <c r="W26" s="25"/>
+      <c r="X26" s="25"/>
+      <c r="Y26" s="26"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="15"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="17"/>
-      <c r="P27" s="28"/>
-      <c r="Q27" s="29"/>
-      <c r="R27" s="29"/>
-      <c r="S27" s="16"/>
-      <c r="T27" s="29"/>
-      <c r="U27" s="29"/>
-      <c r="V27" s="29"/>
-      <c r="W27" s="29"/>
-      <c r="X27" s="29"/>
-      <c r="Y27" s="30"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="16"/>
+      <c r="P27" s="27"/>
+      <c r="Q27" s="28"/>
+      <c r="R27" s="28"/>
+      <c r="S27" s="15"/>
+      <c r="T27" s="28"/>
+      <c r="U27" s="28"/>
+      <c r="V27" s="28"/>
+      <c r="W27" s="28"/>
+      <c r="X27" s="28"/>
+      <c r="Y27" s="29"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -1373,57 +1379,59 @@
       <c r="C29" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="14"/>
-      <c r="P29" s="25"/>
-      <c r="Q29" s="26"/>
-      <c r="R29" s="26"/>
-      <c r="S29" s="26"/>
-      <c r="T29" s="13"/>
-      <c r="U29" s="26"/>
-      <c r="V29" s="26"/>
-      <c r="W29" s="26"/>
-      <c r="X29" s="26"/>
-      <c r="Y29" s="27"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="13"/>
+      <c r="P29" s="24"/>
+      <c r="Q29" s="25"/>
+      <c r="R29" s="25"/>
+      <c r="S29" s="25"/>
+      <c r="T29" s="12"/>
+      <c r="U29" s="25"/>
+      <c r="V29" s="25"/>
+      <c r="W29" s="25"/>
+      <c r="X29" s="25"/>
+      <c r="Y29" s="26"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="17"/>
-      <c r="P30" s="28"/>
-      <c r="Q30" s="29"/>
-      <c r="R30" s="29"/>
-      <c r="S30" s="29"/>
-      <c r="T30" s="16"/>
-      <c r="U30" s="29"/>
-      <c r="V30" s="29"/>
-      <c r="W30" s="29"/>
-      <c r="X30" s="29"/>
-      <c r="Y30" s="30"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="16"/>
+      <c r="P30" s="27"/>
+      <c r="Q30" s="28"/>
+      <c r="R30" s="28"/>
+      <c r="S30" s="28"/>
+      <c r="T30" s="15"/>
+      <c r="U30" s="28"/>
+      <c r="V30" s="28"/>
+      <c r="W30" s="28"/>
+      <c r="X30" s="28"/>
+      <c r="Y30" s="29"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="32" t="s">
+      <c r="E33" s="31" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1431,7 +1439,7 @@
       <c r="C34" t="s">
         <v>19</v>
       </c>
-      <c r="E34" s="32" t="s">
+      <c r="E34" s="31" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1439,7 +1447,7 @@
       <c r="C35" t="s">
         <v>21</v>
       </c>
-      <c r="E35" s="32" t="s">
+      <c r="E35" s="31" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1447,7 +1455,7 @@
       <c r="C36" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="32" t="s">
+      <c r="E36" s="31" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1455,7 +1463,7 @@
       <c r="C37" t="s">
         <v>31</v>
       </c>
-      <c r="E37" s="32" t="s">
+      <c r="E37" s="31" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1463,24 +1471,29 @@
       <c r="C38" t="s">
         <v>35</v>
       </c>
-      <c r="E38" s="32" t="s">
+      <c r="E38" s="31" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E39" s="32"/>
+      <c r="C39" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" s="31" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E40" s="32"/>
+      <c r="E40" s="31"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E41" s="32"/>
+      <c r="E41" s="31"/>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E42" s="32"/>
+      <c r="E42" s="31"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E43" s="32"/>
+      <c r="E43" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>